<commit_message>
Updating Assembly Manual and BOM
</commit_message>
<xml_diff>
--- a/Manual/PCB LGR BOM Rev1.0.xlsx
+++ b/Manual/PCB LGR BOM Rev1.0.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\Exchange\Projects\0079 CPF-NIGM-0079 ODNP resonator\System Components\Loop-gap resonator\Phase II\PCB LGR\Manual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\tkeller\Repositories\OpenPCBLGR\Manual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1E3AF940-D285-4BC0-B8FA-64F251EA6323}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D48198C-5F3A-4615-9072-994F675FE344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{93230D16-BCCB-4C11-9440-E15493A7B9C5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>BOM for PCB LGR</t>
   </si>
@@ -182,6 +182,18 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/remington-industries/30SNSP-125/11614448</t>
+  </si>
+  <si>
+    <t>2057-RF1-106-D-00-50-HDW-ND</t>
+  </si>
+  <si>
+    <t>BNC STRAIGHT BULKHEAD SKT 50 OHM</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/en/products/detail/adam-tech/RF1-106-D-00-50-HDW/9830449</t>
+  </si>
+  <si>
+    <t>Total Cost:</t>
   </si>
 </sst>
 </file>
@@ -538,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32C6D9C5-3E01-4B6C-9E8C-914FD4D1E519}">
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,6 +572,13 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="2">
+        <f>SUM(G:G)</f>
+        <v>139.17959999999997</v>
+      </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -642,7 +661,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2">
-        <f t="shared" ref="G7:G22" si="0">E7*F7</f>
+        <f t="shared" ref="G7:G23" si="0">E7*F7</f>
         <v>1</v>
       </c>
     </row>
@@ -1033,6 +1052,33 @@
       </c>
       <c r="H22" s="2" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>18</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="2">
+        <v>1.48</v>
+      </c>
+      <c r="G23" s="2">
+        <f t="shared" si="0"/>
+        <v>1.48</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>